<commit_message>
Monte Carlo and Sensitivity Updates:
Added new Monte Carlo format where users input distributions of parameters directly instead of perturbations of input variables

Expanded Sensitivity/Monte Carlo support for parameters introduced into temoatools in recent updates i.e. CostInvestIncr

Applied Monte Carlo simulation tecniques to emerging_tech project
</commit_message>
<xml_diff>
--- a/examples/baselines/data/sensitivityVariables.xlsx
+++ b/examples/baselines/data/sensitivityVariables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jab6ft\PycharmProjects\temoatools\examples\puerto_rico_stoch\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\PycharmProjects\coopercenter_temoatools\projects\test_emerging_tech\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950E596A-38E3-4C5F-97C8-FC07F301C99E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="3"/>
+    <workbookView xWindow="31050" yWindow="1800" windowWidth="23250" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
   <si>
     <t>variable</t>
   </si>
@@ -90,12 +91,36 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>CostInvestIncr</t>
+  </si>
+  <si>
+    <t>CostFixedIncr</t>
+  </si>
+  <si>
+    <t>CapacityCredit</t>
+  </si>
+  <si>
+    <t>StorageDuration</t>
+  </si>
+  <si>
+    <t>HeatRate</t>
+  </si>
+  <si>
+    <t>LastBuild</t>
+  </si>
+  <si>
+    <t>FirstBuild</t>
+  </si>
+  <si>
+    <t>Retirement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -150,6 +175,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,19 +455,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -449,15 +475,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -465,7 +491,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -473,7 +499,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -487,20 +513,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -508,141 +534,205 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -651,20 +741,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -672,61 +762,85 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -735,20 +849,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -756,36 +870,76 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>